<commit_message>
Biomass upload finished, started aquapac
</commit_message>
<xml_diff>
--- a/analysis/SERD_Files_Mapping.xlsx
+++ b/analysis/SERD_Files_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{48FA2476-D73C-4244-B65D-A11DB5C025E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7E35009A-2BD4-47D7-9464-5733E43E257A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{48FA2476-D73C-4244-B65D-A11DB5C025E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{C419E5B4-0D4A-4A59-9024-951E798AF7A8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" activeTab="1" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="5" r:id="rId1"/>
@@ -893,17 +893,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -943,9 +934,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -955,9 +943,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -982,6 +967,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1299,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF416807-1578-4EC3-8E4D-DB242418A5D2}">
   <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="7" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="38" t="s">
         <v>219</v>
       </c>
     </row>
@@ -1347,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216DE2DC-4331-4218-BF29-460195BF954E}">
   <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:I24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1368,7 @@
       <c r="A1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="32" t="s">
         <v>154</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -1377,38 +1377,38 @@
       <c r="E1" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="42"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E2" s="10" t="s">
+      <c r="D2" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="H2" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="10" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1416,25 +1416,25 @@
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E3" s="10" t="s">
+      <c r="C3" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="17">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="10" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1442,25 +1442,25 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="17">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1468,25 +1468,25 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="D5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="17">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="I5" s="10" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1494,25 +1494,25 @@
       <c r="A6" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="D6" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="17">
         <v>5</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1520,25 +1520,25 @@
       <c r="A7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="17">
         <v>6</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="I7" s="12" t="s">
+      <c r="I7" s="10" t="s">
         <v>132</v>
       </c>
     </row>
@@ -1546,25 +1546,25 @@
       <c r="A8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="C8" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="17">
         <v>7</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1572,25 +1572,25 @@
       <c r="A9" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E9" s="10" t="s">
+      <c r="C9" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="17">
         <v>8</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="I9" s="12" t="s">
+      <c r="I9" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1598,25 +1598,25 @@
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E10" s="10" t="s">
+      <c r="C10" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="17">
         <v>9</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="H10" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1624,25 +1624,25 @@
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E11" s="10" t="s">
+      <c r="C11" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="17">
         <v>10</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="H11" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1650,25 +1650,25 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="C12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="20">
+      <c r="G12" s="17">
         <v>11</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="10" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1676,25 +1676,25 @@
       <c r="A13" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="C13" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="20">
+      <c r="G13" s="17">
         <v>12</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="10" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1702,25 +1702,25 @@
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="C14" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="17">
         <v>13</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="I14" s="10" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1728,25 +1728,25 @@
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="11" t="s">
+      <c r="F15" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="20">
+      <c r="G15" s="17">
         <v>14</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="10" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1754,21 +1754,21 @@
       <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="14" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="17">
         <v>15</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="H16" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="I16" s="10" t="s">
         <v>143</v>
       </c>
     </row>
@@ -1776,25 +1776,25 @@
       <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="C17" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F17" s="11" t="s">
+      <c r="F17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="20">
+      <c r="G17" s="17">
         <v>16</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H17" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="I17" s="10" t="s">
         <v>145</v>
       </c>
     </row>
@@ -1802,25 +1802,25 @@
       <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="C18" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G18" s="20">
+      <c r="G18" s="17">
         <v>17</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H18" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="I18" s="10" t="s">
         <v>140</v>
       </c>
     </row>
@@ -1828,210 +1828,210 @@
       <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G19" s="20">
+      <c r="G19" s="17">
         <v>18</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="10" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
+      <c r="A20" s="30" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="17">
         <v>19</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="I20" s="12" t="s">
+      <c r="I20" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
+      <c r="A21" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11" t="s">
+      <c r="B21" s="30"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="17">
         <v>20</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="H21" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="I21" s="12" t="s">
+      <c r="I21" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+      <c r="A22" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="35"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="17">
         <v>21</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="A23" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="35"/>
-      <c r="C23" s="9" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="G23" s="20">
+      <c r="G23" s="17">
         <v>22</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="H23" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="I23" s="10" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="17" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="19">
         <v>23</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="I24" s="18" t="s">
+      <c r="I24" s="16" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="30"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="30"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="30"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="30"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="30"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="A30" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="30"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="30"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="30"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="A33" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="35"/>
+      <c r="B33" s="30"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+      <c r="A34" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="35"/>
+      <c r="B34" s="30"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="35"/>
+      <c r="B35" s="30"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+      <c r="A36" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="35"/>
+      <c r="B36" s="30"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="35" t="s">
+      <c r="A37" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="35"/>
+      <c r="B37" s="30"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2197,1337 +2197,1355 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2748F7A6-9708-4A82-9ADC-4118F011AC82}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="23" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="40"/>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="20">
+      <c r="C2" s="24"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="G2" s="20">
+      <c r="H2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="J2" s="20">
+      <c r="K2" s="17">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="20">
+      <c r="C3" s="24"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="17">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G3" s="20">
+      <c r="H3" s="17">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J3" s="20">
+      <c r="K3" s="17">
         <v>2</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="20">
+      <c r="C4" s="24"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="17">
         <v>3</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="G4" s="20">
+      <c r="H4" s="17">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="20">
+      <c r="K4" s="17">
         <v>3</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="M4" s="10" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="20">
+      <c r="E5" s="17">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="G5" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G5" s="20">
+      <c r="H5" s="17">
         <v>4</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="I5" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="J5" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J5" s="20">
+      <c r="K5" s="17">
         <v>4</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="L5" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="20">
+      <c r="E6" s="17">
         <v>5</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="20">
+      <c r="H6" s="17">
         <v>5</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="J6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J6" s="20">
+      <c r="K6" s="17">
         <v>5</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="L6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="20">
+      <c r="C7" s="24"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="17">
         <v>6</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G7" s="20">
+      <c r="H7" s="17">
         <v>18</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J7" s="20">
+      <c r="K7" s="17">
         <v>8</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="29"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="20">
+      <c r="C8" s="24"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="17">
         <v>7</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G8" s="20">
+      <c r="H8" s="17">
         <v>22</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="I8" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="J8" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J8" s="20">
+      <c r="K8" s="17">
         <v>7</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="L8" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="M8" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="20">
+      <c r="C9" s="24"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="17">
         <v>8</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="G9" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="G9" s="20">
+      <c r="H9" s="17">
         <v>21</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="J9" s="20">
+      <c r="K9" s="17">
         <v>14</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="M9" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="20">
+      <c r="C10" s="24"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="17">
         <v>9</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="G10" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="G10" s="20">
+      <c r="H10" s="17">
         <v>15</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="J10" s="20">
+      <c r="K10" s="17">
         <v>11</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="L10" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="M10" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="29"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="20">
+      <c r="C11" s="24"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="17">
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="G11" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G11" s="20">
+      <c r="H11" s="17">
         <v>17</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="J11" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J11" s="20">
+      <c r="K11" s="17">
         <v>22</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="L11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="M11" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="20">
+      <c r="C12" s="24"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="17">
         <v>11</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="F12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="G12" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G12" s="20">
+      <c r="H12" s="17">
         <v>19</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="J12" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J12" s="20">
+      <c r="K12" s="17">
         <v>19</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="M12" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="29"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="20">
+      <c r="C13" s="24"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="17">
         <v>12</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H13" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="I13" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K13" s="36" t="s">
+      <c r="H13" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I13" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K13" s="20" t="s">
         <v>197</v>
       </c>
       <c r="L13" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="29"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="20">
+      <c r="C14" s="24"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="17">
         <v>13</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="F14" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="G14" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="G14" s="20">
+      <c r="H14" s="17">
         <v>9</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="I14" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="J14" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="J14" s="20">
+      <c r="K14" s="17">
         <v>12</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="L14" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="M14" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="29"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="20">
+      <c r="C15" s="24"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="17">
         <v>14</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="F15" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="G15" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="G15" s="20">
+      <c r="H15" s="17">
         <v>7</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="I15" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="I15" s="21" t="s">
+      <c r="J15" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="J15" s="20">
+      <c r="K15" s="17">
         <v>9</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="L15" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="L15" s="13" t="s">
+      <c r="M15" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="29"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="20">
+      <c r="C16" s="24"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="17">
         <v>15</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="F16" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="G16" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="G16" s="20">
+      <c r="H16" s="17">
         <v>13</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="I16" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="21" t="s">
+      <c r="J16" s="18" t="s">
         <v>173</v>
       </c>
-      <c r="J16" s="20">
+      <c r="K16" s="17">
         <v>21</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="L16" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L16" s="13" t="s">
+      <c r="M16" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="20">
+      <c r="C17" s="24"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="17">
         <v>16</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="F17" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="G17" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G17" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H17" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="I17" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K17" s="36" t="s">
+      <c r="H17" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K17" s="20" t="s">
         <v>197</v>
       </c>
       <c r="L17" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="29"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="20">
+      <c r="C18" s="24"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="17">
         <v>17</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="F18" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="G18" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="20">
+      <c r="H18" s="17">
         <v>10</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="I18" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="I18" s="21" t="s">
+      <c r="J18" s="18" t="s">
         <v>176</v>
       </c>
-      <c r="J18" s="20">
+      <c r="K18" s="17">
         <v>13</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="L18" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="L18" s="13" t="s">
+      <c r="M18" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="29"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="20">
+      <c r="C19" s="24"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="17">
         <v>18</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="G19" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="G19" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="I19" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K19" s="36" t="s">
+      <c r="H19" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I19" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K19" s="20" t="s">
         <v>197</v>
       </c>
       <c r="L19" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="20">
+      <c r="C20" s="24"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="17">
         <v>19</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="F20" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="G20" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G20" s="20">
+      <c r="H20" s="17">
         <v>12</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="I20" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="I20" s="21" t="s">
+      <c r="J20" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J20" s="20">
+      <c r="K20" s="17">
         <v>18</v>
       </c>
-      <c r="K20" s="12" t="s">
+      <c r="L20" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="L20" s="13" t="s">
+      <c r="M20" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="20">
+      <c r="C21" s="24"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="17">
         <v>20</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="F21" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F21" s="21" t="s">
+      <c r="G21" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="G21" s="20">
+      <c r="H21" s="17">
         <v>11</v>
       </c>
-      <c r="H21" s="12" t="s">
+      <c r="I21" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="I21" s="21" t="s">
+      <c r="J21" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="J21" s="20">
+      <c r="K21" s="17">
         <v>17</v>
       </c>
-      <c r="K21" s="12" t="s">
+      <c r="L21" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="M21" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="20">
+      <c r="B22" s="30"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="17">
         <v>21</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="F22" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="G22" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G22" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H22" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="I22" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K22" s="36" t="s">
+      <c r="H22" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I22" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J22" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K22" s="20" t="s">
         <v>197</v>
       </c>
       <c r="L22" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
+      <c r="M22" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="20">
+      <c r="B23" s="30"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="17">
         <v>22</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="F23" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="F23" s="21" t="s">
+      <c r="G23" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G23" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H23" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J23" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K23" s="36" t="s">
+      <c r="H23" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I23" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J23" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K23" s="20" t="s">
         <v>197</v>
       </c>
       <c r="L23" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="M23" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="20">
+      <c r="B24" s="30"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="17">
         <v>23</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="F24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="G24" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="20">
+      <c r="H24" s="17">
         <v>14</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="I24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I24" s="21" t="s">
+      <c r="J24" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J24" s="20">
+      <c r="K24" s="17">
         <v>16</v>
       </c>
-      <c r="K24" s="12" t="s">
+      <c r="L24" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L24" s="13" t="s">
+      <c r="M24" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>23</v>
       </c>
       <c r="B25" s="30"/>
       <c r="C25" s="25"/>
-      <c r="D25" s="20">
+      <c r="D25" s="21"/>
+      <c r="E25" s="17">
         <v>24</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="F25" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="G25" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G25" s="20">
+      <c r="H25" s="17">
         <v>16</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="I25" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="I25" s="21" t="s">
+      <c r="J25" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J25" s="20">
+      <c r="K25" s="17">
         <v>15</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="L25" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="L25" s="13" t="s">
+      <c r="M25" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B26" s="30"/>
       <c r="C26" s="25"/>
-      <c r="D26" s="20">
+      <c r="D26" s="21"/>
+      <c r="E26" s="17">
         <v>25</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="F26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="G26" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G26" s="20">
+      <c r="H26" s="17">
         <v>20</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="I26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="I26" s="21" t="s">
+      <c r="J26" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J26" s="20">
+      <c r="K26" s="17">
         <v>6</v>
       </c>
-      <c r="K26" s="12" t="s">
+      <c r="L26" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L26" s="13" t="s">
+      <c r="M26" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
         <v>25</v>
       </c>
       <c r="B27" s="30"/>
       <c r="C27" s="25"/>
-      <c r="D27" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="G27" s="20">
+      <c r="D27" s="21"/>
+      <c r="E27" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F27" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H27" s="17">
         <v>6</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="I27" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="I27" s="21" t="s">
+      <c r="J27" s="18" t="s">
         <v>171</v>
       </c>
-      <c r="J27" s="20">
+      <c r="K27" s="17">
         <v>20</v>
       </c>
-      <c r="K27" s="12" t="s">
+      <c r="L27" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="L27" s="13" t="s">
+      <c r="M27" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="30"/>
       <c r="C28" s="25"/>
-      <c r="D28" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="E28" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="20">
+      <c r="D28" s="21"/>
+      <c r="E28" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="F28" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G28" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="17">
         <v>8</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="I28" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="I28" s="21" t="s">
+      <c r="J28" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="J28" s="20">
+      <c r="K28" s="17">
         <v>10</v>
       </c>
-      <c r="K28" s="12" t="s">
+      <c r="L28" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="M28" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="30"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="20">
+      <c r="D29" s="21"/>
+      <c r="E29" s="17">
         <v>26</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="F29" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="F29" s="21" t="s">
+      <c r="G29" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G29" s="20">
+      <c r="H29" s="17">
         <v>23</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="I29" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="I29" s="21" t="s">
+      <c r="J29" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J29" s="20">
+      <c r="K29" s="17">
         <v>23</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="L29" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="M29" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="30"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="20">
+      <c r="D30" s="21"/>
+      <c r="E30" s="17">
         <v>27</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="F30" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="G30" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G30" s="20">
+      <c r="H30" s="17">
         <v>24</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="I30" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="I30" s="21" t="s">
+      <c r="J30" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J30" s="20">
+      <c r="K30" s="17">
         <v>24</v>
       </c>
-      <c r="K30" s="12" t="s">
+      <c r="L30" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="L30" s="13" t="s">
+      <c r="M30" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="30"/>
       <c r="C31" s="25"/>
-      <c r="D31" s="20">
+      <c r="D31" s="21"/>
+      <c r="E31" s="17">
         <v>28</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="F31" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="F31" s="21" t="s">
+      <c r="G31" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G31" s="20">
+      <c r="H31" s="17">
         <v>25</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="I31" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="I31" s="21" t="s">
+      <c r="J31" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J31" s="20">
+      <c r="K31" s="17">
         <v>25</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="L31" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="L31" s="13" t="s">
+      <c r="M31" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="30"/>
       <c r="C32" s="25"/>
-      <c r="D32" s="20">
+      <c r="D32" s="21"/>
+      <c r="E32" s="17">
         <v>29</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="F32" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="G32" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="20">
+      <c r="H32" s="17">
         <v>26</v>
       </c>
-      <c r="H32" s="12" t="s">
+      <c r="I32" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="I32" s="21" t="s">
+      <c r="J32" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J32" s="20">
+      <c r="K32" s="17">
         <v>26</v>
       </c>
-      <c r="K32" s="12" t="s">
+      <c r="L32" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="L32" s="13" t="s">
+      <c r="M32" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="30"/>
       <c r="C33" s="25"/>
-      <c r="D33" s="20">
+      <c r="D33" s="21"/>
+      <c r="E33" s="17">
         <v>30</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="F33" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="G33" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G33" s="20">
+      <c r="H33" s="17">
         <v>27</v>
       </c>
-      <c r="H33" s="12" t="s">
+      <c r="I33" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="I33" s="21" t="s">
+      <c r="J33" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J33" s="20">
+      <c r="K33" s="17">
         <v>27</v>
       </c>
-      <c r="K33" s="12" t="s">
+      <c r="L33" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="L33" s="13" t="s">
+      <c r="M33" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="30" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="30"/>
       <c r="C34" s="25"/>
-      <c r="D34" s="20">
+      <c r="D34" s="21"/>
+      <c r="E34" s="17">
         <v>31</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="F34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="G34" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G34" s="20">
+      <c r="H34" s="17">
         <v>28</v>
       </c>
-      <c r="H34" s="12" t="s">
+      <c r="I34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="21" t="s">
+      <c r="J34" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J34" s="20">
+      <c r="K34" s="17">
         <v>28</v>
       </c>
-      <c r="K34" s="12" t="s">
+      <c r="L34" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="L34" s="13" t="s">
+      <c r="M34" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="25"/>
-      <c r="D35" s="20">
+      <c r="D35" s="21"/>
+      <c r="E35" s="17">
         <v>32</v>
       </c>
-      <c r="E35" s="12" t="s">
+      <c r="F35" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="G35" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G35" s="20">
+      <c r="H35" s="17">
         <v>29</v>
       </c>
-      <c r="H35" s="12" t="s">
+      <c r="I35" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="J35" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J35" s="20">
+      <c r="K35" s="17">
         <v>29</v>
       </c>
-      <c r="K35" s="12" t="s">
+      <c r="L35" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="L35" s="13" t="s">
+      <c r="M35" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="35" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B36" s="30"/>
       <c r="C36" s="25"/>
-      <c r="D36" s="20">
+      <c r="D36" s="21"/>
+      <c r="E36" s="17">
         <v>33</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="F36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="G36" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G36" s="20">
+      <c r="H36" s="17">
         <v>30</v>
       </c>
-      <c r="H36" s="12" t="s">
+      <c r="I36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="J36" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J36" s="20">
+      <c r="K36" s="17">
         <v>30</v>
       </c>
-      <c r="K36" s="12" t="s">
+      <c r="L36" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="L36" s="13" t="s">
+      <c r="M36" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="35" t="s">
+    <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="32"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="23">
+      <c r="B37" s="30"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="19">
         <v>34</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="F37" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="F37" s="34" t="s">
+      <c r="G37" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="G37" s="23">
+      <c r="H37" s="19">
         <v>31</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="I37" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="I37" s="34" t="s">
+      <c r="J37" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="J37" s="23">
+      <c r="K37" s="19">
         <v>31</v>
       </c>
-      <c r="K37" s="18" t="s">
+      <c r="L37" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="L37" s="19" t="s">
+      <c r="M37" s="16" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="35" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="30" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="30"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -3629,9 +3647,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3640,819 +3658,838 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B55925D-514D-40B6-9C15-4DD8370C08AF}">
-  <dimension ref="A1:L67"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="36" t="s">
         <v>214</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="E1" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="39" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="22" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="40"/>
+      <c r="M1" s="42"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="C2" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="D2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="29">
+      <c r="E2" s="24">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="G2" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="G2" s="20">
+      <c r="H2" s="17">
         <v>1</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="J2" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="20">
+      <c r="K2" s="17">
         <v>1</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="C3" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D3" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="29">
+      <c r="E3" s="24">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="20">
+      <c r="H3" s="17">
         <v>2</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="J3" s="20">
+      <c r="K3" s="17">
         <v>2</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="M3" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="C4" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="D4" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="29">
+      <c r="E4" s="24">
         <v>3</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="20">
+      <c r="H4" s="17">
         <v>3</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="J4" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L4" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M4" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="C5" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="D5" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D5" s="29">
+      <c r="E5" s="24">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="G5" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="I5" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L5" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J5" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="C6" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="29">
+      <c r="E6" s="24">
         <v>5</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G6" s="20">
+      <c r="H6" s="17">
         <v>6</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="I6" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="J6" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="J6" s="20">
+      <c r="K6" s="17">
         <v>4</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="L6" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="M6" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="C7" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="D7" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="29">
+      <c r="E7" s="24">
         <v>6</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="G7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="20">
+      <c r="H7" s="17">
         <v>5</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="I7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="21" t="s">
+      <c r="J7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="J7" s="20">
+      <c r="K7" s="17">
         <v>3</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="L7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="M7" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="C8" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="D8" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D8" s="29">
+      <c r="E8" s="24">
         <v>7</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="G8" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="I8" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L8" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="C9" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="29">
+      <c r="E9" s="24">
         <v>8</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="G9" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G9" s="20">
+      <c r="H9" s="17">
         <v>9</v>
       </c>
-      <c r="H9" s="12" t="s">
+      <c r="I9" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="J9" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="20">
+      <c r="K9" s="17">
         <v>5</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="L9" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="M9" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="C10" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="29">
+      <c r="E10" s="24">
         <v>9</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="F10" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="G10" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G10" s="20">
+      <c r="H10" s="17">
         <v>7</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="I10" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J10" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L10" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M10" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="C11" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="29">
+      <c r="E11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="F11" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="G11" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G11" s="20">
+      <c r="H11" s="17">
         <v>10</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="I11" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="I11" s="21" t="s">
+      <c r="J11" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L11" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="C12" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="D12" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D12" s="29">
+      <c r="E12" s="24">
         <v>11</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="F12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="G12" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G12" s="20">
+      <c r="H12" s="17">
         <v>8</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="J12" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J12" s="20">
+      <c r="K12" s="17">
         <v>6</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="L12" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="M12" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="C13" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="D13" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="D13" s="29">
+      <c r="E13" s="24">
         <v>12</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="G13" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="G13" s="20">
+      <c r="H13" s="17">
         <v>11</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="I13" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="I13" s="21" t="s">
+      <c r="J13" s="18" t="s">
         <v>161</v>
       </c>
-      <c r="J13" s="24" t="s">
-        <v>197</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="L13" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="20" t="s">
+        <v>197</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="M13" s="26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="C14" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="D14" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="D14" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="27" t="s">
         <v>197</v>
       </c>
       <c r="F14" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="H14" s="19">
         <v>4</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="I14" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="J14" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="J14" s="39" t="s">
-        <v>197</v>
-      </c>
-      <c r="K14" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="L14" s="40" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14" s="34" t="s">
+        <v>197</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>197</v>
+      </c>
+      <c r="M14" s="35" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="35"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="B24" s="30"/>
+      <c r="F24" s="30"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="35" t="s">
+      <c r="B25" s="30"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="B26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="B27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
+      <c r="B28" s="30"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="B29" s="30"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="35" t="s">
+      <c r="B30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
+      <c r="B31" s="30"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35" t="s">
+      <c r="B32" s="30"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="30" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" s="30"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="35" t="s">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="30" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" s="30"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4982,6 +5019,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -5204,27 +5261,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB90D271-0391-4568-AFE8-0F0AB2F87BD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5241,29 +5303,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
only_one_instrument adde to UPLOAD_SERD_UTIL
</commit_message>
<xml_diff>
--- a/analysis/SERD_Files_Mapping.xlsx
+++ b/analysis/SERD_Files_Mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evri.sharepoint.com/sites/ukho-meds/Shared Documents/MEDS DB/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="6_{0C145658-17D9-4227-B73F-1B16731E47F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E4EFC81F-F098-4CA8-8F24-5259F3440581}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="6_{0C145658-17D9-4227-B73F-1B16731E47F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E61AF461-C0E3-4A80-BB5A-9D4DE9E95DD5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
   </bookViews>
   <sheets>
     <sheet name="PROFILE_INDEX" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="183">
   <si>
     <t>RECORDNUMBER</t>
   </si>
@@ -559,9 +559,6 @@
   </si>
   <si>
     <t>position 47</t>
-  </si>
-  <si>
-    <t>Waiting algorithm</t>
   </si>
   <si>
     <t>SHIP_DETAIL.MEDS_SHIP_NUMBER</t>
@@ -586,7 +583,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,8 +599,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +618,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -890,10 +899,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1039,8 +1049,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1355,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216DE2DC-4331-4218-BF29-460195BF954E}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,7 +1436,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>74</v>
@@ -1445,7 +1465,7 @@
         <v>2</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>76</v>
@@ -1465,15 +1485,17 @@
         <v>148</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G4" s="17">
         <v>3</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="I4" s="9" t="s">
         <v>78</v>
       </c>
@@ -1501,7 +1523,7 @@
         <v>4</v>
       </c>
       <c r="H5" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>66</v>
@@ -1529,11 +1551,11 @@
       <c r="G6" s="17">
         <v>5</v>
       </c>
-      <c r="H6" s="53"/>
-      <c r="I6" s="9" t="s">
+      <c r="H6" s="65"/>
+      <c r="I6" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="67" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1557,7 +1579,7 @@
         <v>6</v>
       </c>
       <c r="H7" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>69</v>
@@ -1586,7 +1608,7 @@
         <v>7</v>
       </c>
       <c r="H8" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>84</v>
@@ -1615,7 +1637,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>85</v>
@@ -1644,7 +1666,7 @@
         <v>9</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>87</v>
@@ -1673,7 +1695,7 @@
         <v>10</v>
       </c>
       <c r="H11" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>88</v>
@@ -1702,7 +1724,7 @@
         <v>11</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>89</v>
@@ -1731,7 +1753,7 @@
         <v>12</v>
       </c>
       <c r="H13" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>68</v>
@@ -1760,7 +1782,7 @@
         <v>13</v>
       </c>
       <c r="H14" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I14" s="9" t="s">
         <v>7</v>
@@ -1789,7 +1811,7 @@
         <v>14</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I15" s="9" t="s">
         <v>92</v>
@@ -1812,7 +1834,7 @@
         <v>15</v>
       </c>
       <c r="H16" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>93</v>
@@ -1825,9 +1847,15 @@
       <c r="A17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="C17" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="F17" s="52" t="s">
         <v>12</v>
       </c>
@@ -1835,7 +1863,7 @@
         <v>16</v>
       </c>
       <c r="H17" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>95</v>
@@ -1864,7 +1892,7 @@
         <v>17</v>
       </c>
       <c r="H18" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>97</v>
@@ -1877,9 +1905,15 @@
       <c r="A19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+      <c r="C19" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>146</v>
+      </c>
       <c r="F19" s="8" t="s">
         <v>176</v>
       </c>
@@ -1887,7 +1921,7 @@
         <v>18</v>
       </c>
       <c r="H19" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>98</v>
@@ -1901,16 +1935,24 @@
         <v>57</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="8" t="s">
-        <v>177</v>
+      <c r="C20" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20" s="52" t="s">
+        <v>6</v>
       </c>
       <c r="G20" s="17">
         <v>19</v>
       </c>
-      <c r="H20" s="53"/>
+      <c r="H20" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="I20" s="9" t="s">
         <v>99</v>
       </c>
@@ -1923,16 +1965,24 @@
         <v>22</v>
       </c>
       <c r="B21" s="29"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="8" t="s">
-        <v>177</v>
+      <c r="C21" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F21" s="52" t="s">
+        <v>6</v>
       </c>
       <c r="G21" s="17">
         <v>20</v>
       </c>
-      <c r="H21" s="53"/>
+      <c r="H21" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="I21" s="9" t="s">
         <v>101</v>
       </c>
@@ -1945,16 +1995,24 @@
         <v>23</v>
       </c>
       <c r="B22" s="29"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8" t="s">
-        <v>177</v>
+      <c r="C22" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>6</v>
       </c>
       <c r="G22" s="17">
         <v>21</v>
       </c>
-      <c r="H22" s="53"/>
+      <c r="H22" s="53" t="s">
+        <v>179</v>
+      </c>
       <c r="I22" s="9" t="s">
         <v>102</v>
       </c>
@@ -1974,16 +2032,16 @@
         <v>148</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G23" s="17">
         <v>22</v>
       </c>
       <c r="H23" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I23" s="9" t="s">
         <v>103</v>
@@ -1997,9 +2055,15 @@
         <v>3</v>
       </c>
       <c r="B24" s="29"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="C24" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>146</v>
+      </c>
       <c r="F24" s="14" t="s">
         <v>12</v>
       </c>
@@ -2007,7 +2071,7 @@
         <v>23</v>
       </c>
       <c r="H24" s="54" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>104</v>
@@ -2293,7 +2357,7 @@
         <v>147</v>
       </c>
       <c r="E1" s="36" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F1" s="60" t="s">
         <v>143</v>
@@ -2438,7 +2502,7 @@
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>148</v>
@@ -2479,7 +2543,7 @@
         <v>105</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>148</v>
@@ -7331,26 +7395,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -7573,32 +7617,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB90D271-0391-4568-AFE8-0F0AB2F87BD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7615,4 +7654,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
V_STG_SERD_ROW_MAIN updated fixing size of position reference, from 11 to 12
</commit_message>
<xml_diff>
--- a/analysis/SERD_Files_Mapping.xlsx
+++ b/analysis/SERD_Files_Mapping.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="52" documentId="6_{0C145658-17D9-4227-B73F-1B16731E47F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E61AF461-C0E3-4A80-BB5A-9D4DE9E95DD5}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
   </bookViews>
   <sheets>
     <sheet name="PROFILE_INDEX" sheetId="2" r:id="rId1"/>
@@ -1034,6 +1034,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1048,15 +1057,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1375,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216DE2DC-4331-4218-BF29-460195BF954E}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -1409,12 +1409,12 @@
       <c r="F1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="62"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1551,11 +1551,11 @@
       <c r="G6" s="17">
         <v>5</v>
       </c>
-      <c r="H6" s="65"/>
-      <c r="I6" s="66" t="s">
+      <c r="H6" s="60"/>
+      <c r="I6" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="67" t="s">
+      <c r="J6" s="62" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2359,21 +2359,21 @@
       <c r="E1" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="60" t="s">
+      <c r="G1" s="64"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="61"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="60" t="s">
+      <c r="J1" s="64"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="M1" s="61"/>
-      <c r="N1" s="62"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="65"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4059,21 +4059,21 @@
       <c r="D1" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="67" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="60" t="s">
+      <c r="F1" s="64"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="I1" s="61"/>
-      <c r="J1" s="63"/>
-      <c r="K1" s="60" t="s">
+      <c r="I1" s="64"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="L1" s="61"/>
-      <c r="M1" s="62"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="65"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -7395,6 +7395,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -7617,27 +7637,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB90D271-0391-4568-AFE8-0F0AB2F87BD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7654,29 +7679,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOWNLOAD_SERD_UTIL version #1 (SV works fine) done
</commit_message>
<xml_diff>
--- a/analysis/SERD_Files_Mapping.xlsx
+++ b/analysis/SERD_Files_Mapping.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="52" documentId="6_{0C145658-17D9-4227-B73F-1B16731E47F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E61AF461-C0E3-4A80-BB5A-9D4DE9E95DD5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27870" windowHeight="14160" activeTab="3" xr2:uid="{0302A20B-65BC-4FFC-A169-DD929ACADB36}"/>
   </bookViews>
   <sheets>
     <sheet name="PROFILE_INDEX" sheetId="2" r:id="rId1"/>
@@ -1375,8 +1375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{216DE2DC-4331-4218-BF29-460195BF954E}">
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2325,7 +2325,7 @@
   <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4028,7 +4028,7 @@
   <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4866,7 +4866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F060310E-1F88-4686-9470-C12E54B461AB}">
   <dimension ref="A1:KQ19"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3:W3"/>
     </sheetView>
   </sheetViews>
@@ -7395,26 +7395,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CEAE28352B96D64C95AA0D5E2FA62FAD" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ed183881d36ac1b5d7d67982eda510d1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d161086-4829-409f-9f75-5bde88dcb151" xmlns:ns3="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="685f4fda20cf913d28bf77c13cd653dd" ns2:_="" ns3:_="">
     <xsd:import namespace="3d161086-4829-409f-9f75-5bde88dcb151"/>
@@ -7637,32 +7617,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d161086-4829-409f-9f75-5bde88dcb151">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB90D271-0391-4568-AFE8-0F0AB2F87BD2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7679,4 +7654,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E890D57-E472-4BCE-903F-454BDC6E18F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B4520AE-A84B-45D3-BF92-BC546C144CDF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3d161086-4829-409f-9f75-5bde88dcb151"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="42d8e6db-7b1e-4a51-8fbb-e5e83cc76820"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>